<commit_message>
added header and hyperlinks
</commit_message>
<xml_diff>
--- a/secure/captains_contact.xlsx
+++ b/secure/captains_contact.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="24915" windowHeight="12600"/>
+    <workbookView xWindow="690" yWindow="0" windowWidth="24915" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="135">
   <si>
     <t>January, 2018</t>
   </si>
@@ -108,9 +108,6 @@
     <t>604-575-0085</t>
   </si>
   <si>
-    <t xml:space="preserve"> brenda.nordgren@gmail.com</t>
-  </si>
-  <si>
     <t>Fraserview</t>
   </si>
   <si>
@@ -174,9 +171,6 @@
     <t>Marine Drive</t>
   </si>
   <si>
-    <t>Marj Allen &amp; Lynn Nielsen</t>
-  </si>
-  <si>
     <t>604-306-3939</t>
   </si>
   <si>
@@ -406,6 +400,27 @@
   </si>
   <si>
     <t>cindyhehh@hotmail.com</t>
+  </si>
+  <si>
+    <t>brenda.nordgren@gmail.com</t>
+  </si>
+  <si>
+    <t>Golf Club</t>
+  </si>
+  <si>
+    <t>Captain</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Lynn Nielsen</t>
+  </si>
+  <si>
+    <t>Marj Allen</t>
   </si>
 </sst>
 </file>
@@ -459,54 +474,20 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -533,6 +514,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -552,25 +548,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -578,6 +565,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -941,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,499 +952,515 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="12"/>
+      <c r="A1" s="9"/>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13" t="s">
+      <c r="A2" s="9"/>
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
     </row>
     <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
     </row>
     <row r="4" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13" t="s">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-    </row>
-    <row r="5" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13" t="s">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+    </row>
+    <row r="6" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D7" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D8" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D9" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D10" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+    <row r="11" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D11" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D12" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C13" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D13" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="C14" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="D14" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="6" t="s">
+    </row>
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="C15" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="D15" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="6" t="s">
+    </row>
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="C16" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="D16" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="6" t="s">
+    </row>
+    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="C17" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="D17" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="6" t="s">
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="C18" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="D18" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="6" t="s">
+    </row>
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+      <c r="B19" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="D19" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="6" t="s">
+    </row>
+    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3"/>
+      <c r="B20" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="6" t="s">
+    </row>
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6" t="s">
+      <c r="B21" s="4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="D21" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="6" t="s">
+    </row>
+    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="B22" s="4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="D22" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="6" t="s">
+    </row>
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="B23" s="7" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="D23" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C22" s="9" t="s">
+    </row>
+    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="B24" s="4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
+      <c r="C24" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="D24" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C23" s="6" t="s">
+    </row>
+    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="B25" s="13"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="D26" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="6" t="s">
+    </row>
+    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="B27" s="4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="D27" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="6" t="s">
+    </row>
+    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="B28" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="D28" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C27" s="6" t="s">
+    </row>
+    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="B29" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
+      <c r="C29" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="D29" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C28" s="6" t="s">
+    </row>
+    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="B30" s="4" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="D30" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C29" s="6" t="s">
+    </row>
+    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="B31" s="4" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="5" t="s">
+      <c r="C31" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="D31" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C30" s="6" t="s">
+    </row>
+    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="B32" s="13"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
+      <c r="B33" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
+      <c r="C33" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="D33" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C32" s="6" t="s">
+    </row>
+    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="B34" s="4" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="5" t="s">
+      <c r="C34" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="D34" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C33" s="6" t="s">
+    </row>
+    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="B35" s="4" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
+      <c r="C35" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="D35" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="C34" s="6" t="s">
+    </row>
+    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="B36" s="4" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
+      <c r="C36" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="D36" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="C35" s="6" t="s">
+    </row>
+    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="B37" s="4" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="5" t="s">
+      <c r="C37" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="D37" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="C36" s="6" t="s">
+    </row>
+    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="B38" s="4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
+      <c r="C38" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="D38" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="C37" s="6" t="s">
+    </row>
+    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="B39" s="4" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
+      <c r="C39" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="D39" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="C38" s="6" t="s">
+    </row>
+    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="B40" s="4" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
+      <c r="C40" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="D40" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="C39" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1459,11 +1471,42 @@
     <mergeCell ref="B5:D5"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D29" r:id="rId1" display="mailto:crabtalk@gmail.com"/>
+    <hyperlink ref="D30" r:id="rId1"/>
+    <hyperlink ref="D7" r:id="rId2"/>
+    <hyperlink ref="D8" r:id="rId3"/>
+    <hyperlink ref="D9" r:id="rId4"/>
+    <hyperlink ref="D10" r:id="rId5"/>
+    <hyperlink ref="D11" r:id="rId6"/>
+    <hyperlink ref="D12" r:id="rId7"/>
+    <hyperlink ref="D13" r:id="rId8"/>
+    <hyperlink ref="D14" r:id="rId9"/>
+    <hyperlink ref="D15" r:id="rId10"/>
+    <hyperlink ref="D16" r:id="rId11"/>
+    <hyperlink ref="D17" r:id="rId12"/>
+    <hyperlink ref="D18" r:id="rId13"/>
+    <hyperlink ref="D19" r:id="rId14"/>
+    <hyperlink ref="D20" r:id="rId15"/>
+    <hyperlink ref="D21" r:id="rId16"/>
+    <hyperlink ref="D22" r:id="rId17"/>
+    <hyperlink ref="D23" r:id="rId18"/>
+    <hyperlink ref="D24" r:id="rId19"/>
+    <hyperlink ref="D26" r:id="rId20"/>
+    <hyperlink ref="D27" r:id="rId21"/>
+    <hyperlink ref="D28" r:id="rId22"/>
+    <hyperlink ref="D29" r:id="rId23"/>
+    <hyperlink ref="D31" r:id="rId24"/>
+    <hyperlink ref="D33" r:id="rId25"/>
+    <hyperlink ref="D34" r:id="rId26"/>
+    <hyperlink ref="D35" r:id="rId27"/>
+    <hyperlink ref="D36" r:id="rId28"/>
+    <hyperlink ref="D37" r:id="rId29"/>
+    <hyperlink ref="D38" r:id="rId30"/>
+    <hyperlink ref="D39" r:id="rId31"/>
+    <hyperlink ref="D40" r:id="rId32"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId33"/>
+  <drawing r:id="rId34"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
SW added Tsawwassen Tue and fixed pin sheet
</commit_message>
<xml_diff>
--- a/secure/captains_contact.xlsx
+++ b/secure/captains_contact.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
   <si>
     <t>January, 2018</t>
   </si>
@@ -279,18 +279,6 @@
     <t>lomaandstephen@icloud.com</t>
   </si>
   <si>
-    <t>Quilchena BW</t>
-  </si>
-  <si>
-    <t>Casandra Kobayashi</t>
-  </si>
-  <si>
-    <t>604-731-8455</t>
-  </si>
-  <si>
-    <t>crabtalk@gmail.com</t>
-  </si>
-  <si>
     <t>Richmond</t>
   </si>
   <si>
@@ -342,18 +330,6 @@
     <t>bd2006@telus.net</t>
   </si>
   <si>
-    <t>Tsawwassen Springs BW</t>
-  </si>
-  <si>
-    <t>Moira Milligan</t>
-  </si>
-  <si>
-    <t>604-329-0299</t>
-  </si>
-  <si>
-    <t>moira.milligan@gmail.com</t>
-  </si>
-  <si>
     <t>University</t>
   </si>
   <si>
@@ -364,18 +340,6 @@
   </si>
   <si>
     <t>Lindai@shaw.ca</t>
-  </si>
-  <si>
-    <t>University BW</t>
-  </si>
-  <si>
-    <t>Lori Hutchinson</t>
-  </si>
-  <si>
-    <t>778-838-6256</t>
-  </si>
-  <si>
-    <t>lhutchinson11@gmail.com</t>
   </si>
   <si>
     <t>Vancouver</t>
@@ -560,12 +524,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -574,6 +532,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -937,10 +901,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,51 +916,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="9"/>
+      <c r="A1" s="12"/>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="10" t="s">
+      <c r="A2" s="12"/>
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
     </row>
     <row r="4" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="10" t="s">
+      <c r="A4" s="12"/>
+      <c r="B4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
     </row>
     <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
     </row>
     <row r="6" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>132</v>
+      <c r="A6" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1094,7 +1058,7 @@
         <v>29</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1172,7 +1136,7 @@
         <v>50</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>51</v>
@@ -1184,7 +1148,7 @@
     <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="4" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="8" t="s">
@@ -1251,7 +1215,7 @@
       <c r="A25" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B25" s="13"/>
+      <c r="B25" s="11"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
     </row>
@@ -1329,23 +1293,23 @@
       <c r="A31" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>94</v>
-      </c>
+      <c r="B31" s="11"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D32" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B32" s="13"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
     </row>
     <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
@@ -1417,50 +1381,8 @@
         <v>115</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
+    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1471,42 +1393,39 @@
     <mergeCell ref="B5:D5"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D30" r:id="rId1"/>
-    <hyperlink ref="D7" r:id="rId2"/>
-    <hyperlink ref="D8" r:id="rId3"/>
-    <hyperlink ref="D9" r:id="rId4"/>
-    <hyperlink ref="D10" r:id="rId5"/>
-    <hyperlink ref="D11" r:id="rId6"/>
-    <hyperlink ref="D12" r:id="rId7"/>
-    <hyperlink ref="D13" r:id="rId8"/>
-    <hyperlink ref="D14" r:id="rId9"/>
-    <hyperlink ref="D15" r:id="rId10"/>
-    <hyperlink ref="D16" r:id="rId11"/>
-    <hyperlink ref="D17" r:id="rId12"/>
-    <hyperlink ref="D18" r:id="rId13"/>
-    <hyperlink ref="D19" r:id="rId14"/>
-    <hyperlink ref="D20" r:id="rId15"/>
-    <hyperlink ref="D21" r:id="rId16"/>
-    <hyperlink ref="D22" r:id="rId17"/>
-    <hyperlink ref="D23" r:id="rId18"/>
-    <hyperlink ref="D24" r:id="rId19"/>
-    <hyperlink ref="D26" r:id="rId20"/>
-    <hyperlink ref="D27" r:id="rId21"/>
-    <hyperlink ref="D28" r:id="rId22"/>
-    <hyperlink ref="D29" r:id="rId23"/>
-    <hyperlink ref="D31" r:id="rId24"/>
+    <hyperlink ref="D7" r:id="rId1"/>
+    <hyperlink ref="D8" r:id="rId2"/>
+    <hyperlink ref="D9" r:id="rId3"/>
+    <hyperlink ref="D10" r:id="rId4"/>
+    <hyperlink ref="D11" r:id="rId5"/>
+    <hyperlink ref="D12" r:id="rId6"/>
+    <hyperlink ref="D13" r:id="rId7"/>
+    <hyperlink ref="D14" r:id="rId8"/>
+    <hyperlink ref="D15" r:id="rId9"/>
+    <hyperlink ref="D16" r:id="rId10"/>
+    <hyperlink ref="D17" r:id="rId11"/>
+    <hyperlink ref="D18" r:id="rId12"/>
+    <hyperlink ref="D19" r:id="rId13"/>
+    <hyperlink ref="D20" r:id="rId14"/>
+    <hyperlink ref="D21" r:id="rId15"/>
+    <hyperlink ref="D22" r:id="rId16"/>
+    <hyperlink ref="D23" r:id="rId17"/>
+    <hyperlink ref="D24" r:id="rId18"/>
+    <hyperlink ref="D26" r:id="rId19"/>
+    <hyperlink ref="D27" r:id="rId20"/>
+    <hyperlink ref="D28" r:id="rId21"/>
+    <hyperlink ref="D29" r:id="rId22"/>
+    <hyperlink ref="D30" r:id="rId23"/>
+    <hyperlink ref="D32" r:id="rId24"/>
     <hyperlink ref="D33" r:id="rId25"/>
     <hyperlink ref="D34" r:id="rId26"/>
     <hyperlink ref="D35" r:id="rId27"/>
     <hyperlink ref="D36" r:id="rId28"/>
     <hyperlink ref="D37" r:id="rId29"/>
-    <hyperlink ref="D38" r:id="rId30"/>
-    <hyperlink ref="D39" r:id="rId31"/>
-    <hyperlink ref="D40" r:id="rId32"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId33"/>
-  <drawing r:id="rId34"/>
+  <pageSetup orientation="portrait" r:id="rId30"/>
+  <drawing r:id="rId31"/>
 </worksheet>
 </file>
 

</xml_diff>